<commit_message>
working on recommendation notebook
</commit_message>
<xml_diff>
--- a/04_lu_tables/lu_cond_recommendations_2024-07-16.xlsx
+++ b/04_lu_tables/lu_cond_recommendations_2024-07-16.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cassi\Documents\GitHub_AB-RCSC\Jupyter-web-app\04_lu_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABMI_Official\RCDST_Jupyter_webapp_Official\04_lu_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF14BEE4-E190-4D23-9223-85DB868D69F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D00F3D-67E0-43E9-9EE7-5A334829C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{A3A66B7D-82F1-429E-93DA-F36142727237}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A3A66B7D-82F1-429E-93DA-F36142727237}"/>
   </bookViews>
   <sheets>
     <sheet name="rec_sample-design" sheetId="4" r:id="rId1"/>
@@ -5313,125 +5313,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="318">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="151">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5511,106 +5393,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5622,6 +5411,14 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5686,22 +5483,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
           <bgColor rgb="FFF3F3F3"/>
         </patternFill>
@@ -5738,14 +5519,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFD9EAD3"/>
           <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF3F3F3"/>
-          <bgColor rgb="FFF3F3F3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6068,268 +5841,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF2F2F2"/>
@@ -6469,6 +5980,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
@@ -6519,14 +6038,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6854,6 +6365,22 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF2F2F2"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -6924,584 +6451,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFEDE2F6"/>
           <bgColor rgb="FFEDE2F6"/>
         </patternFill>
@@ -7542,286 +6491,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFEF2CB"/>
           <bgColor rgb="FFFEF2CB"/>
         </patternFill>
@@ -7832,6 +6501,22 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFB4C6E7"/>
           <bgColor rgb="FFB4C6E7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFD9"/>
+          <bgColor rgb="FFE2EFD9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDEEAF6"/>
+          <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7862,30 +6547,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2F2F2"/>
-          <bgColor rgb="FFF2F2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEDE2F6"/>
-          <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFBE4D5"/>
           <bgColor rgb="FFFBE4D5"/>
         </patternFill>
@@ -7902,16 +6563,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFDEEAF6"/>
-          <bgColor rgb="FFDEEAF6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
+          <fgColor rgb="FFB4C6E7"/>
+          <bgColor rgb="FFB4C6E7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7926,14 +6579,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFDEEAF6"/>
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
@@ -7942,40 +6587,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFEF2CB"/>
-          <bgColor rgb="FFFEF2CB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB4C6E7"/>
-          <bgColor rgb="FFB4C6E7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFEDE2F6"/>
           <bgColor rgb="FFEDE2F6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFBE4D5"/>
-          <bgColor rgb="FFFBE4D5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFD9"/>
-          <bgColor rgb="FFE2EFD9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -28207,439 +26820,429 @@
   </sheetData>
   <autoFilter ref="A1:T319" xr:uid="{7B6020DB-08C4-4728-9A69-1B986D9EC16D}"/>
   <conditionalFormatting sqref="D112:F164">
-    <cfRule type="cellIs" dxfId="205" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="35" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E254:E319">
-    <cfRule type="cellIs" dxfId="204" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="36" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="containsText" dxfId="203" priority="37" operator="containsText" text="camdays_per_loc">
+    <cfRule type="containsText" dxfId="148" priority="39" operator="containsText" text="num_cams">
+      <formula>NOT(ISERROR(SEARCH(("num_cams"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="147" priority="42" operator="containsText" text="cam_spacing">
+      <formula>NOT(ISERROR(SEARCH(("cam_spacing"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="146" priority="41" operator="containsText" text="cam_days_ttl">
+      <formula>NOT(ISERROR(SEARCH(("cam_days_ttl"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="145" priority="40" operator="containsText" text="survey_duration">
+      <formula>NOT(ISERROR(SEARCH(("survey_duration"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="144" priority="37" operator="containsText" text="camdays_per_loc">
       <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(G1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="38" operator="containsText" text="cam_arrange">
+    <cfRule type="containsText" dxfId="143" priority="38" operator="containsText" text="cam_arrange">
       <formula>NOT(ISERROR(SEARCH(("cam_arrange"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="201" priority="39" operator="containsText" text="num_cams">
-      <formula>NOT(ISERROR(SEARCH(("num_cams"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="40" operator="containsText" text="survey_duration">
-      <formula>NOT(ISERROR(SEARCH(("survey_duration"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="41" operator="containsText" text="cam_days_ttl">
-      <formula>NOT(ISERROR(SEARCH(("cam_days_ttl"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="42" operator="containsText" text="cam_spacing">
-      <formula>NOT(ISERROR(SEARCH(("cam_spacing"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G319">
-    <cfRule type="containsText" dxfId="197" priority="43" operator="containsText" text="Survey duration">
+    <cfRule type="containsText" dxfId="142" priority="49" operator="containsText" text="Number of cameras">
+      <formula>NOT(ISERROR(SEARCH(("Number of cameras"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="141" priority="48" operator="containsText" text="Camera arrangement">
+      <formula>NOT(ISERROR(SEARCH(("Camera arrangement"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="140" priority="47" operator="containsText" text="Camera days per camera location">
+      <formula>NOT(ISERROR(SEARCH(("Camera days per camera location"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="139" priority="46" operator="containsText" text="Camera spacing">
+      <formula>NOT(ISERROR(SEARCH(("Camera spacing"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="138" priority="45" operator="containsText" text="camdays_per_loc">
+      <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(G1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="137" priority="43" operator="containsText" text="Survey duration">
       <formula>NOT(ISERROR(SEARCH(("Survey duration"),(G1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="44" operator="containsText" text="Total number of camera days">
+    <cfRule type="containsText" dxfId="136" priority="44" operator="containsText" text="Total number of camera days">
       <formula>NOT(ISERROR(SEARCH(("Total number of camera days"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="195" priority="45" operator="containsText" text="camdays_per_loc">
-      <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="46" operator="containsText" text="Camera spacing">
-      <formula>NOT(ISERROR(SEARCH(("Camera spacing"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="47" operator="containsText" text="Camera days per camera location">
-      <formula>NOT(ISERROR(SEARCH(("Camera days per camera location"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="48" operator="containsText" text="Camera arrangement">
-      <formula>NOT(ISERROR(SEARCH(("Camera arrangement"),(G1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="49" operator="containsText" text="Number of cameras">
-      <formula>NOT(ISERROR(SEARCH(("Number of cameras"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G64:G213">
-    <cfRule type="cellIs" dxfId="190" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="50" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G254:G319 P254:P272 O254:O299 R254:R319">
-    <cfRule type="cellIs" dxfId="189" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="51" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H319">
-    <cfRule type="containsText" dxfId="188" priority="52" operator="containsText" text="num_cams">
+    <cfRule type="containsText" dxfId="133" priority="54" operator="containsText" text="camdays_per_loc">
+      <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(H1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="53" operator="containsText" text="cam_arrange">
+      <formula>NOT(ISERROR(SEARCH(("cam_arrange"),(H1))))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="131" priority="52" operator="containsText" text="num_cams">
       <formula>NOT(ISERROR(SEARCH(("num_cams"),(H1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="53" operator="containsText" text="cam_arrange">
-      <formula>NOT(ISERROR(SEARCH(("cam_arrange"),(H1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="186" priority="54" operator="containsText" text="camdays_per_loc">
-      <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(H1))))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="55" operator="containsText" text="survey_duration">
+    <cfRule type="containsText" dxfId="130" priority="55" operator="containsText" text="survey_duration">
       <formula>NOT(ISERROR(SEARCH(("survey_duration"),(H1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="56" operator="containsText" text="cam_days_ttl">
+    <cfRule type="containsText" dxfId="129" priority="56" operator="containsText" text="cam_days_ttl">
       <formula>NOT(ISERROR(SEARCH(("cam_days_ttl"),(H1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="57" operator="containsText" text="cam_spacing">
+    <cfRule type="containsText" dxfId="128" priority="57" operator="containsText" text="cam_spacing">
       <formula>NOT(ISERROR(SEARCH(("cam_spacing"),(H1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="182" priority="33" operator="containsText" text="hr_size">
+    <cfRule type="containsText" dxfId="127" priority="33" operator="containsText" text="hr_size">
       <formula>NOT(ISERROR(SEARCH("hr_size",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I26 I28:I29 I32:I39 I41:I63">
-    <cfRule type="cellIs" dxfId="181" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="58" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I152:I164">
-    <cfRule type="cellIs" dxfId="180" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="59" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I255:I272 I274:I275 I277 I280 I283:I288 I290:I293 I295:I299 I301:I303 I305:I317 I319">
-    <cfRule type="cellIs" dxfId="179" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="60" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="containsText" dxfId="178" priority="34" operator="containsText" text="hr_size">
+    <cfRule type="containsText" dxfId="123" priority="34" operator="containsText" text="hr_size">
       <formula>NOT(ISERROR(SEARCH("hr_size",L1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P128">
-    <cfRule type="cellIs" dxfId="177" priority="61" operator="equal">
+  <conditionalFormatting sqref="M113:M115 M152:M153 M158:M161 M292">
+    <cfRule type="cellIs" dxfId="122" priority="16" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N319">
-    <cfRule type="cellIs" dxfId="164" priority="74" operator="equal">
+  <conditionalFormatting sqref="M117:M119">
+    <cfRule type="cellIs" dxfId="121" priority="1" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M127:M135">
+    <cfRule type="cellIs" dxfId="120" priority="2" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M137:M143">
+    <cfRule type="cellIs" dxfId="119" priority="15" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M145">
+    <cfRule type="cellIs" dxfId="118" priority="3" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M196">
+    <cfRule type="cellIs" dxfId="117" priority="4" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M200:M201">
+    <cfRule type="cellIs" dxfId="116" priority="5" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M208:M209">
+    <cfRule type="cellIs" dxfId="115" priority="6" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M212">
+    <cfRule type="cellIs" dxfId="114" priority="7" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M214:M215">
+    <cfRule type="cellIs" dxfId="113" priority="8" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M217">
+    <cfRule type="cellIs" dxfId="112" priority="9" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M219">
+    <cfRule type="cellIs" dxfId="111" priority="10" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M221">
+    <cfRule type="cellIs" dxfId="110" priority="11" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M224:M225">
+    <cfRule type="cellIs" dxfId="109" priority="12" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M227:M228">
+    <cfRule type="cellIs" dxfId="108" priority="13" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:N319">
+    <cfRule type="cellIs" dxfId="107" priority="14" operator="equal">
       <formula>"min"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N143">
-    <cfRule type="cellIs" dxfId="163" priority="75" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="cellIs" dxfId="162" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="76" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:N31">
-    <cfRule type="cellIs" dxfId="161" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="77" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N35">
-    <cfRule type="cellIs" dxfId="160" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="78" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N41">
-    <cfRule type="cellIs" dxfId="159" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="79" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46:N47">
-    <cfRule type="cellIs" dxfId="158" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="80" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52">
-    <cfRule type="cellIs" dxfId="157" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="81" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55">
-    <cfRule type="cellIs" dxfId="156" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="82" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N58">
-    <cfRule type="cellIs" dxfId="155" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="83" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N115:N116">
-    <cfRule type="cellIs" dxfId="154" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="84" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N122">
-    <cfRule type="cellIs" dxfId="153" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="85" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N126:N129">
-    <cfRule type="cellIs" dxfId="152" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N131:N132">
-    <cfRule type="cellIs" dxfId="151" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="87" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N136:N137">
-    <cfRule type="cellIs" dxfId="150" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="88" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N144">
-    <cfRule type="cellIs" dxfId="149" priority="89" operator="equal">
+  <conditionalFormatting sqref="N143:N144">
+    <cfRule type="cellIs" dxfId="93" priority="75" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N158">
-    <cfRule type="cellIs" dxfId="148" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N161:N162">
-    <cfRule type="cellIs" dxfId="147" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N269">
-    <cfRule type="cellIs" dxfId="146" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N273">
-    <cfRule type="cellIs" dxfId="145" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N289">
-    <cfRule type="cellIs" dxfId="144" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="94" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N299">
-    <cfRule type="cellIs" dxfId="143" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="95" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N303">
-    <cfRule type="cellIs" dxfId="142" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="96" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N307:N309">
-    <cfRule type="cellIs" dxfId="141" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="97" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N312">
-    <cfRule type="cellIs" dxfId="140" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="98" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N315">
-    <cfRule type="cellIs" dxfId="139" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="99" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N318">
-    <cfRule type="cellIs" dxfId="138" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="100" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O63">
-    <cfRule type="cellIs" dxfId="137" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="101" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O319">
-    <cfRule type="containsText" dxfId="136" priority="102" operator="containsText" text="stratified">
+    <cfRule type="containsText" dxfId="80" priority="102" operator="containsText" text="stratified">
       <formula>NOT(ISERROR(SEARCH(("stratified"),(O1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O112:O164">
-    <cfRule type="cellIs" dxfId="135" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="103" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O182">
-    <cfRule type="cellIs" dxfId="134" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="104" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O300:P319 I112:I150 P1 N140">
-    <cfRule type="cellIs" dxfId="133" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="105" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1">
-    <cfRule type="cellIs" dxfId="132" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="106" operator="equal">
       <formula>"NA [concepts]"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="107" operator="equal">
       <formula>"[need to input]"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="P128">
+    <cfRule type="cellIs" dxfId="74" priority="61" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="P274:P307">
-    <cfRule type="cellIs" dxfId="130" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="108" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1">
-    <cfRule type="containsText" dxfId="129" priority="109" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="72" priority="109" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH(("TRUE"),(Q1))))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="110" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q63">
-    <cfRule type="cellIs" dxfId="127" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="111" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q164">
-    <cfRule type="containsText" dxfId="126" priority="112" operator="containsText" text="MAYBE">
+    <cfRule type="containsText" dxfId="69" priority="112" operator="containsText" text="MAYBE">
       <formula>NOT(ISERROR(SEARCH(("MAYBE"),(Q1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q64:Q164">
-    <cfRule type="containsText" dxfId="125" priority="113" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="68" priority="113" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH(("TRUE"),(Q64))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q165:Q213">
-    <cfRule type="containsText" dxfId="124" priority="114" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="67" priority="114" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH(("maybe"),(Q165))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="115" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="66" priority="115" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH(("TRUE"),(Q165))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q214:Q253">
-    <cfRule type="containsText" dxfId="122" priority="116" operator="containsText" text="MAYBE">
+    <cfRule type="containsText" dxfId="65" priority="116" operator="containsText" text="MAYBE">
       <formula>NOT(ISERROR(SEARCH(("MAYBE"),(Q214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q214:Q319">
-    <cfRule type="containsText" dxfId="121" priority="117" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="64" priority="117" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH(("TRUE"),(Q214))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q254:Q319">
-    <cfRule type="containsText" dxfId="120" priority="118" operator="containsText" text="MAYBE">
+    <cfRule type="containsText" dxfId="63" priority="118" operator="containsText" text="MAYBE">
       <formula>NOT(ISERROR(SEARCH(("MAYBE"),(Q254))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R40">
-    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="119" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R46:R63">
-    <cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="120" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R96">
-    <cfRule type="cellIs" dxfId="117" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="121" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R112:R129">
-    <cfRule type="cellIs" dxfId="116" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="122" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R131:R164">
-    <cfRule type="cellIs" dxfId="115" priority="123" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M117:M119">
-    <cfRule type="cellIs" dxfId="98" priority="1" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M127:M135">
-    <cfRule type="cellIs" dxfId="97" priority="2" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M145">
-    <cfRule type="cellIs" dxfId="96" priority="3" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M196">
-    <cfRule type="cellIs" dxfId="95" priority="4" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M200:M201">
-    <cfRule type="cellIs" dxfId="94" priority="5" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M208:M209">
-    <cfRule type="cellIs" dxfId="93" priority="6" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M212">
-    <cfRule type="cellIs" dxfId="92" priority="7" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M214:M215">
-    <cfRule type="cellIs" dxfId="91" priority="8" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M217">
-    <cfRule type="cellIs" dxfId="90" priority="9" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M219">
-    <cfRule type="cellIs" dxfId="89" priority="10" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M221">
-    <cfRule type="cellIs" dxfId="88" priority="11" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M224:M225">
-    <cfRule type="cellIs" dxfId="87" priority="12" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M227:M228">
-    <cfRule type="cellIs" dxfId="86" priority="13" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M319">
-    <cfRule type="cellIs" dxfId="85" priority="14" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M143">
-    <cfRule type="cellIs" dxfId="84" priority="15" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M113:M115 M137:M142 M152:M153 M158:M161 M292">
-    <cfRule type="cellIs" dxfId="83" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="123" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28655,9 +27258,9 @@
   </sheetPr>
   <dimension ref="A1:AI1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -31272,125 +29875,125 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="G2:H2 O2:P9 O11:O27 P13">
-    <cfRule type="cellIs" dxfId="82" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:H7 G9:G18">
-    <cfRule type="cellIs" dxfId="81" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:I3 K3:L3">
-    <cfRule type="cellIs" dxfId="80" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9:H10">
-    <cfRule type="cellIs" dxfId="79" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:J18">
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:L14">
-    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16:L16">
-    <cfRule type="cellIs" dxfId="76" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="containsText" dxfId="75" priority="8" operator="containsText" text="sp_size">
+    <cfRule type="containsText" dxfId="50" priority="8" operator="containsText" text="sp_size">
       <formula>NOT(ISERROR(SEARCH(("sp_size"),(P2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="9" operator="containsText" text="rarity">
+    <cfRule type="containsText" dxfId="49" priority="9" operator="containsText" text="rarity">
       <formula>NOT(ISERROR(SEARCH(("rarity"),(P2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="10" operator="containsText" text="sp_size">
+    <cfRule type="containsText" dxfId="48" priority="10" operator="containsText" text="sp_size">
       <formula>NOT(ISERROR(SEARCH(("sp_size"),(P2))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="rarity">
+    <cfRule type="containsText" dxfId="47" priority="11" operator="containsText" text="rarity">
       <formula>NOT(ISERROR(SEARCH(("rarity"),(P2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4">
-    <cfRule type="containsText" dxfId="71" priority="12" operator="containsText" text="sp_size">
+    <cfRule type="containsText" dxfId="46" priority="12" operator="containsText" text="sp_size">
       <formula>NOT(ISERROR(SEARCH(("sp_size"),(P4))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="rarity">
+    <cfRule type="containsText" dxfId="45" priority="13" operator="containsText" text="rarity">
       <formula>NOT(ISERROR(SEARCH(("rarity"),(P4))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5:P8 X1:X27">
-    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="sp_size">
+    <cfRule type="containsText" dxfId="44" priority="14" operator="containsText" text="sp_size">
       <formula>NOT(ISERROR(SEARCH(("sp_size"),(P5))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P13">
-    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="sp_size">
+    <cfRule type="containsText" dxfId="43" priority="15" operator="containsText" text="sp_size">
       <formula>NOT(ISERROR(SEARCH(("sp_size"),(P13))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="rarity">
+    <cfRule type="containsText" dxfId="42" priority="16" operator="containsText" text="rarity">
       <formula>NOT(ISERROR(SEARCH(("rarity"),(P13))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R17">
-    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U20 V21 U22:U27">
-    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="Survey duration">
+    <cfRule type="containsText" dxfId="40" priority="18" operator="containsText" text="Survey duration">
       <formula>NOT(ISERROR(SEARCH(("Survey duration"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="19" operator="containsText" text="Total number of camera days">
+    <cfRule type="containsText" dxfId="39" priority="19" operator="containsText" text="Total number of camera days">
       <formula>NOT(ISERROR(SEARCH(("Total number of camera days"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="camdays_per_loc">
+    <cfRule type="containsText" dxfId="38" priority="20" operator="containsText" text="camdays_per_loc">
       <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="Camera spacing">
+    <cfRule type="containsText" dxfId="37" priority="21" operator="containsText" text="Camera spacing">
       <formula>NOT(ISERROR(SEARCH(("Camera spacing"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="Camera days per camera location">
+    <cfRule type="containsText" dxfId="36" priority="22" operator="containsText" text="Camera days per camera location">
       <formula>NOT(ISERROR(SEARCH(("Camera days per camera location"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="23" operator="containsText" text="Camera arrangement">
+    <cfRule type="containsText" dxfId="35" priority="23" operator="containsText" text="Camera arrangement">
       <formula>NOT(ISERROR(SEARCH(("Camera arrangement"),(U1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="24" operator="containsText" text="Number of cameras">
+    <cfRule type="containsText" dxfId="34" priority="24" operator="containsText" text="Number of cameras">
       <formula>NOT(ISERROR(SEARCH(("Number of cameras"),(U1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1:V27">
-    <cfRule type="containsText" dxfId="58" priority="25" operator="containsText" text="num_cams">
+    <cfRule type="containsText" dxfId="33" priority="25" operator="containsText" text="num_cams">
       <formula>NOT(ISERROR(SEARCH(("num_cams"),(V1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="26" operator="containsText" text="cam_arrange">
+    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="cam_arrange">
       <formula>NOT(ISERROR(SEARCH(("cam_arrange"),(V1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="27" operator="containsText" text="camdays_per_loc">
+    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="camdays_per_loc">
       <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(V1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="survey_duration">
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="survey_duration">
       <formula>NOT(ISERROR(SEARCH(("survey_duration"),(V1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="29" operator="containsText" text="cam_days_ttl">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="cam_days_ttl">
       <formula>NOT(ISERROR(SEARCH(("cam_days_ttl"),(V1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="30" operator="containsText" text="cam_spacing">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="cam_spacing">
       <formula>NOT(ISERROR(SEARCH(("cam_spacing"),(V1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:X27 P5:P8">
-    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="rarity">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="rarity">
       <formula>NOT(ISERROR(SEARCH(("rarity"),(P5))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33994,44 +32597,39 @@
     <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="B1:F54" xr:uid="{A09229B9-6295-49B2-8C83-1E1F9DC8CECF}"/>
-  <conditionalFormatting sqref="A7:A15 F7:F12 F14:F15 C2:C19 D2:E16 E17:E28">
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A17:A28">
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A41:A54">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1 D17:D28 F17:F28">
-    <cfRule type="cellIs" dxfId="46" priority="9" operator="equal">
+  <conditionalFormatting sqref="C1">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="45" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41:F54">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+  <conditionalFormatting sqref="D2:E16 C2:C19 A7:A15 F7:F15 D17:F28">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+  <conditionalFormatting sqref="D41:F54">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34047,7 +32645,7 @@
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
@@ -46265,122 +44863,85 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="B1:K319" xr:uid="{539D7193-359E-4FE5-B66A-E8F772103EFA}"/>
-  <conditionalFormatting sqref="I254:I280 I283:I319 I1 I96 I112:I129 I131:I164 I46:I63 F28:G29 F32:G39 F41:G63 F2:G26 F152:G164 F255:G272 F274:G275 F277:G277 F280:G280 F283:G288 F290:G293 F295:G299 F301:G303 F305:G317 F319:G319 F112:G150 D112:D164 A112:A164 G3:G319 I12 I15:I40">
-    <cfRule type="cellIs" dxfId="42" priority="30" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J254:J270 I281:I282 J277:J299">
-    <cfRule type="cellIs" dxfId="41" priority="46" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E1:E319">
-    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="num_cams">
+    <cfRule type="containsText" dxfId="18" priority="47" operator="containsText" text="num_cams">
       <formula>NOT(ISERROR(SEARCH(("num_cams"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="48" operator="containsText" text="cam_arrange">
+    <cfRule type="containsText" dxfId="17" priority="48" operator="containsText" text="cam_arrange">
       <formula>NOT(ISERROR(SEARCH(("cam_arrange"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="49" operator="containsText" text="camdays_per_loc">
+    <cfRule type="containsText" dxfId="16" priority="49" operator="containsText" text="camdays_per_loc">
       <formula>NOT(ISERROR(SEARCH(("camdays_per_loc"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="50" operator="containsText" text="survey_duration">
+    <cfRule type="containsText" dxfId="15" priority="50" operator="containsText" text="survey_duration">
       <formula>NOT(ISERROR(SEARCH(("survey_duration"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="51" operator="containsText" text="cam_days_ttl">
+    <cfRule type="containsText" dxfId="14" priority="51" operator="containsText" text="cam_days_ttl">
       <formula>NOT(ISERROR(SEARCH(("cam_days_ttl"),(E1))))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="52" operator="containsText" text="cam_spacing">
+    <cfRule type="containsText" dxfId="13" priority="52" operator="containsText" text="cam_spacing">
       <formula>NOT(ISERROR(SEARCH(("cam_spacing"),(E1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="34" priority="28" operator="containsText" text="hr_size">
+    <cfRule type="containsText" dxfId="12" priority="28" operator="containsText" text="hr_size">
       <formula>NOT(ISERROR(SEARCH("hr_size",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G26 G3:G319 F28:G29 F32:G39 F41:G63 F112:G150 F152:G164 F255:G272 F274:G275 F277:G277 F280:G280 F283:G288 F290:G293 F295:G299 F301:G303 F305:G317 F319:G319 I1 I12 I15:I40 I46:I63 I96 I112:I129 A112:A164 D112:D164 I131:I164 I254:I319">
+    <cfRule type="cellIs" dxfId="11" priority="30" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I11">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"min"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:I14">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"min"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I79">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J1:J63">
-    <cfRule type="cellIs" dxfId="18" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="96" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J270 J277:J319">
-    <cfRule type="containsText" dxfId="17" priority="97" operator="containsText" text="stratified">
+    <cfRule type="containsText" dxfId="6" priority="97" operator="containsText" text="stratified">
       <formula>NOT(ISERROR(SEARCH(("stratified"),(J1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J112:J164">
-    <cfRule type="cellIs" dxfId="16" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="98" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J182">
-    <cfRule type="cellIs" dxfId="15" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="99" operator="equal">
+      <formula>"-"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J254:J270 J277:J299">
+    <cfRule type="cellIs" dxfId="3" priority="46" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J300:J319">
-    <cfRule type="cellIs" dxfId="14" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="100" operator="equal">
       <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I79">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
-      <formula>"-"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"min"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"min"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="stratified">
       <formula>NOT(ISERROR(SEARCH(("stratified"),(L1))))</formula>
     </cfRule>

</xml_diff>